<commit_message>
added finetuning and evaluation llama2-chat
</commit_message>
<xml_diff>
--- a/notes/Milestones and targets.xlsx
+++ b/notes/Milestones and targets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CyThIA\CyThIA\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDUCATION\THESIS\code\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD96C67-2CBA-4628-A3AF-3FAB17BB4C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAA026B-A2C5-4A46-86EE-79AD53B2B701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{60A02A94-784F-4C39-9C5C-A18761C48642}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{60A02A94-784F-4C39-9C5C-A18761C48642}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Sl No</t>
   </si>
@@ -552,22 +552,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1E9F11-A3D3-42F3-A740-383A93303558}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="3" max="3" width="63.1796875" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" customWidth="1"/>
+    <col min="6" max="6" width="29.26953125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="35.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -611,7 +611,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -630,7 +630,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -640,14 +640,16 @@
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="9">
         <v>1.0482060185185185</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -664,7 +666,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -681,7 +683,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -698,7 +700,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -713,7 +715,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -724,7 +726,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -735,7 +737,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -746,7 +748,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -757,7 +759,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -768,7 +770,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -779,7 +781,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -790,7 +792,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>